<commit_message>
Added database schema in sql format and added index.php
</commit_message>
<xml_diff>
--- a/webservice/push_notification_db.xlsx
+++ b/webservice/push_notification_db.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>username</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Column names</t>
   </si>
   <si>
-    <t>device_type</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -90,12 +87,6 @@
     <t>preferences</t>
   </si>
   <si>
-    <t>preference_id</t>
-  </si>
-  <si>
-    <t>preference_name</t>
-  </si>
-  <si>
     <t>preference title</t>
   </si>
   <si>
@@ -117,13 +108,25 @@
     <t>primary key (preference_id) of preferences table</t>
   </si>
   <si>
-    <t>preference_value</t>
-  </si>
-  <si>
     <t>bool</t>
   </si>
   <si>
     <t xml:space="preserve">either 1 or 0, assuming that values preference will be either 1 or 0 </t>
+  </si>
+  <si>
+    <t>os_type</t>
+  </si>
+  <si>
+    <t>unique_id</t>
+  </si>
+  <si>
+    <t>pref_id</t>
+  </si>
+  <si>
+    <t>pref_name</t>
+  </si>
+  <si>
+    <t>pref_value</t>
   </si>
 </sst>
 </file>
@@ -191,13 +194,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -520,30 +523,30 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -555,15 +558,15 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -575,15 +578,15 @@
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="4"/>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -595,15 +598,15 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -615,15 +618,15 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="A6" s="4"/>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -635,15 +638,15 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -655,7 +658,7 @@
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="4"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -694,17 +697,17 @@
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>23</v>
+      <c r="A11" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -716,15 +719,15 @@
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -764,17 +767,17 @@
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -786,15 +789,15 @@
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -806,15 +809,15 @@
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="5"/>
       <c r="B17" s="2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -826,15 +829,15 @@
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>

</xml_diff>